<commit_message>
added bmi field and message index on workout part
</commit_message>
<xml_diff>
--- a/utils/ProfileSDK126.xlsx
+++ b/utils/ProfileSDK126.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\github\Trainalytics\fit-parse-csv\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D39522-C69B-49C4-A1AE-7CAD55C82F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB3651E-9B4F-44DA-BA08-1E2CDD252D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47025,8 +47025,8 @@
   <dimension ref="A1:P1524"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A997" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1013" sqref="D1013"/>
+      <pane ySplit="1" topLeftCell="A1192" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1202" sqref="D1202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67165,24 +67165,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="1200" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1200" s="9"/>
-      <c r="B1200" s="10">
+    <row r="1200" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1200" s="13"/>
+      <c r="B1200" s="14">
         <v>254</v>
       </c>
-      <c r="C1200" s="9" t="s">
+      <c r="C1200" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="D1200" s="9" t="s">
+      <c r="D1200" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="F1200" s="9"/>
-      <c r="G1200" s="9"/>
-      <c r="J1200" s="9"/>
-      <c r="L1200" s="9"/>
-      <c r="M1200" s="9"/>
-      <c r="N1200" s="9"/>
-      <c r="P1200" s="10">
+      <c r="F1200" s="13"/>
+      <c r="G1200" s="13"/>
+      <c r="J1200" s="13"/>
+      <c r="L1200" s="13"/>
+      <c r="M1200" s="13"/>
+      <c r="N1200" s="13"/>
+      <c r="P1200" s="14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added tank_summary + sleep_assessment section
</commit_message>
<xml_diff>
--- a/utils/ProfileSDK126.xlsx
+++ b/utils/ProfileSDK126.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\github\Trainalytics\fit-parse-csv\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D58AF2B-72A8-49C6-B3D1-DD2FC7C5278B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FA03E5-E568-49F4-A142-4336E366E278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47025,8 +47025,8 @@
   <dimension ref="A1:P1524"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1361" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1370" sqref="C1370"/>
+      <pane ySplit="1" topLeftCell="A1499" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1498" sqref="D1498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -70421,173 +70421,173 @@
         <v>4874</v>
       </c>
     </row>
-    <row r="1391" spans="1:16" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1391" s="11" t="s">
+    <row r="1391" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1391" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="C1391" s="11"/>
-      <c r="D1391" s="11"/>
-      <c r="F1391" s="11"/>
-      <c r="G1391" s="11"/>
-      <c r="J1391" s="11"/>
-      <c r="L1391" s="11"/>
-      <c r="M1391" s="11"/>
-      <c r="N1391" s="11"/>
-    </row>
-    <row r="1392" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1392" s="9"/>
-      <c r="B1392" s="10">
+      <c r="C1391" s="13"/>
+      <c r="D1391" s="13"/>
+      <c r="F1391" s="13"/>
+      <c r="G1391" s="13"/>
+      <c r="J1391" s="13"/>
+      <c r="L1391" s="13"/>
+      <c r="M1391" s="13"/>
+      <c r="N1391" s="13"/>
+    </row>
+    <row r="1392" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1392" s="13"/>
+      <c r="B1392" s="14">
         <v>0</v>
       </c>
-      <c r="C1392" s="9" t="s">
+      <c r="C1392" s="13" t="s">
         <v>4875</v>
       </c>
-      <c r="D1392" s="9" t="s">
+      <c r="D1392" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F1392" s="9"/>
-      <c r="G1392" s="9"/>
-      <c r="J1392" s="9"/>
-      <c r="L1392" s="9"/>
-      <c r="M1392" s="9"/>
-      <c r="N1392" s="9" t="s">
+      <c r="F1392" s="13"/>
+      <c r="G1392" s="13"/>
+      <c r="J1392" s="13"/>
+      <c r="L1392" s="13"/>
+      <c r="M1392" s="13"/>
+      <c r="N1392" s="13" t="s">
         <v>4876</v>
       </c>
     </row>
-    <row r="1393" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1393" s="9"/>
-      <c r="B1393" s="10">
+    <row r="1393" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1393" s="13"/>
+      <c r="B1393" s="14">
         <v>2</v>
       </c>
-      <c r="C1393" s="9" t="s">
+      <c r="C1393" s="13" t="s">
         <v>4877</v>
       </c>
-      <c r="D1393" s="9" t="s">
+      <c r="D1393" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1393" s="9"/>
-      <c r="G1393" s="9">
+      <c r="F1393" s="13"/>
+      <c r="G1393" s="13">
         <v>10</v>
       </c>
-      <c r="I1393" s="10" t="s">
+      <c r="I1393" s="14" t="s">
         <v>4878</v>
       </c>
-      <c r="J1393" s="9"/>
-      <c r="L1393" s="9"/>
-      <c r="M1393" s="9"/>
-      <c r="N1393" s="9"/>
-    </row>
-    <row r="1394" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1394" s="9"/>
-      <c r="B1394" s="10">
+      <c r="J1393" s="13"/>
+      <c r="L1393" s="13"/>
+      <c r="M1393" s="13"/>
+      <c r="N1393" s="13"/>
+    </row>
+    <row r="1394" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1394" s="13"/>
+      <c r="B1394" s="14">
         <v>5</v>
       </c>
-      <c r="C1394" s="9" t="s">
+      <c r="C1394" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1394" s="9" t="s">
+      <c r="D1394" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F1394" s="9"/>
-      <c r="G1394" s="9"/>
-      <c r="J1394" s="9"/>
-      <c r="L1394" s="9"/>
-      <c r="M1394" s="9"/>
-      <c r="N1394" s="9"/>
-    </row>
-    <row r="1395" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1395" s="9"/>
-      <c r="B1395" s="10">
+      <c r="F1394" s="13"/>
+      <c r="G1394" s="13"/>
+      <c r="J1394" s="13"/>
+      <c r="L1394" s="13"/>
+      <c r="M1394" s="13"/>
+      <c r="N1394" s="13"/>
+    </row>
+    <row r="1395" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1395" s="13"/>
+      <c r="B1395" s="14">
         <v>6</v>
       </c>
-      <c r="C1395" s="9" t="s">
+      <c r="C1395" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="D1395" s="9" t="s">
+      <c r="D1395" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="F1395" s="9"/>
-      <c r="G1395" s="9"/>
-      <c r="J1395" s="9"/>
-      <c r="L1395" s="9"/>
-      <c r="M1395" s="9"/>
-      <c r="N1395" s="9"/>
-    </row>
-    <row r="1396" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1396" s="9"/>
-      <c r="B1396" s="10">
+      <c r="F1395" s="13"/>
+      <c r="G1395" s="13"/>
+      <c r="J1395" s="13"/>
+      <c r="L1395" s="13"/>
+      <c r="M1395" s="13"/>
+      <c r="N1395" s="13"/>
+    </row>
+    <row r="1396" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1396" s="13"/>
+      <c r="B1396" s="14">
         <v>8</v>
       </c>
-      <c r="C1396" s="9" t="s">
+      <c r="C1396" s="13" t="s">
         <v>2369</v>
       </c>
-      <c r="D1396" s="9" t="s">
+      <c r="D1396" s="13" t="s">
         <v>2369</v>
       </c>
-      <c r="F1396" s="9"/>
-      <c r="G1396" s="9"/>
-      <c r="J1396" s="9"/>
-      <c r="L1396" s="9"/>
-      <c r="M1396" s="9"/>
-      <c r="N1396" s="9"/>
-    </row>
-    <row r="1397" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1397" s="9"/>
-      <c r="B1397" s="10">
+      <c r="F1396" s="13"/>
+      <c r="G1396" s="13"/>
+      <c r="J1396" s="13"/>
+      <c r="L1396" s="13"/>
+      <c r="M1396" s="13"/>
+      <c r="N1396" s="13"/>
+    </row>
+    <row r="1397" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1397" s="13"/>
+      <c r="B1397" s="14">
         <v>9</v>
       </c>
-      <c r="C1397" s="9" t="s">
+      <c r="C1397" s="13" t="s">
         <v>4879</v>
       </c>
-      <c r="D1397" s="9" t="s">
+      <c r="D1397" s="13" t="s">
         <v>3875</v>
       </c>
-      <c r="F1397" s="9"/>
-      <c r="G1397" s="9"/>
-      <c r="J1397" s="9"/>
-      <c r="L1397" s="9"/>
-      <c r="M1397" s="9"/>
-      <c r="N1397" s="9" t="s">
+      <c r="F1397" s="13"/>
+      <c r="G1397" s="13"/>
+      <c r="J1397" s="13"/>
+      <c r="L1397" s="13"/>
+      <c r="M1397" s="13"/>
+      <c r="N1397" s="13" t="s">
         <v>4880</v>
       </c>
     </row>
-    <row r="1398" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1398" s="9"/>
-      <c r="B1398" s="10">
+    <row r="1398" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1398" s="13"/>
+      <c r="B1398" s="14">
         <v>12</v>
       </c>
-      <c r="C1398" s="9" t="s">
+      <c r="C1398" s="13" t="s">
         <v>4881</v>
       </c>
-      <c r="D1398" s="9" t="s">
+      <c r="D1398" s="13" t="s">
         <v>3787</v>
       </c>
-      <c r="F1398" s="9"/>
-      <c r="G1398" s="9"/>
-      <c r="J1398" s="9"/>
-      <c r="L1398" s="9"/>
-      <c r="M1398" s="9"/>
-      <c r="N1398" s="9" t="s">
+      <c r="F1398" s="13"/>
+      <c r="G1398" s="13"/>
+      <c r="J1398" s="13"/>
+      <c r="L1398" s="13"/>
+      <c r="M1398" s="13"/>
+      <c r="N1398" s="13" t="s">
         <v>4882</v>
       </c>
     </row>
-    <row r="1399" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1399" s="9"/>
-      <c r="B1399" s="10">
+    <row r="1399" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1399" s="13"/>
+      <c r="B1399" s="14">
         <v>13</v>
       </c>
-      <c r="C1399" s="9" t="s">
+      <c r="C1399" s="13" t="s">
         <v>3943</v>
       </c>
-      <c r="D1399" s="9" t="s">
+      <c r="D1399" s="13" t="s">
         <v>3785</v>
       </c>
-      <c r="F1399" s="9"/>
-      <c r="G1399" s="9"/>
-      <c r="J1399" s="9"/>
-      <c r="L1399" s="9"/>
-      <c r="M1399" s="9"/>
-      <c r="N1399" s="9" t="s">
+      <c r="F1399" s="13"/>
+      <c r="G1399" s="13"/>
+      <c r="J1399" s="13"/>
+      <c r="L1399" s="13"/>
+      <c r="M1399" s="13"/>
+      <c r="N1399" s="13" t="s">
         <v>4883</v>
       </c>
     </row>
@@ -70706,57 +70706,57 @@
         <v>4893</v>
       </c>
     </row>
-    <row r="1408" spans="1:16" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1408" s="11" t="s">
+    <row r="1408" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1408" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="C1408" s="11"/>
-      <c r="D1408" s="11"/>
-      <c r="F1408" s="11"/>
-      <c r="G1408" s="11"/>
-      <c r="J1408" s="11"/>
-      <c r="L1408" s="11"/>
-      <c r="M1408" s="11"/>
-      <c r="N1408" s="11"/>
-    </row>
-    <row r="1409" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1409" s="9"/>
-      <c r="B1409" s="10">
+      <c r="C1408" s="13"/>
+      <c r="D1408" s="13"/>
+      <c r="F1408" s="13"/>
+      <c r="G1408" s="13"/>
+      <c r="J1408" s="13"/>
+      <c r="L1408" s="13"/>
+      <c r="M1408" s="13"/>
+      <c r="N1408" s="13"/>
+    </row>
+    <row r="1409" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1409" s="13"/>
+      <c r="B1409" s="14">
         <v>253</v>
       </c>
-      <c r="C1409" s="9" t="s">
+      <c r="C1409" s="13" t="s">
         <v>3829</v>
       </c>
-      <c r="D1409" s="9" t="s">
+      <c r="D1409" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F1409" s="9"/>
-      <c r="G1409" s="9"/>
-      <c r="I1409" s="10" t="s">
+      <c r="F1409" s="13"/>
+      <c r="G1409" s="13"/>
+      <c r="I1409" s="14" t="s">
         <v>3830</v>
       </c>
-      <c r="J1409" s="9"/>
-      <c r="L1409" s="9"/>
-      <c r="M1409" s="9"/>
-      <c r="N1409" s="9"/>
-    </row>
-    <row r="1410" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1410" s="9"/>
-      <c r="B1410" s="10">
+      <c r="J1409" s="13"/>
+      <c r="L1409" s="13"/>
+      <c r="M1409" s="13"/>
+      <c r="N1409" s="13"/>
+    </row>
+    <row r="1410" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1410" s="13"/>
+      <c r="B1410" s="14">
         <v>0</v>
       </c>
-      <c r="C1410" s="9" t="s">
+      <c r="C1410" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D1410" s="9" t="s">
+      <c r="D1410" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F1410" s="9"/>
-      <c r="G1410" s="9"/>
-      <c r="J1410" s="9"/>
-      <c r="L1410" s="9"/>
-      <c r="M1410" s="9"/>
-      <c r="N1410" s="9"/>
+      <c r="F1410" s="13"/>
+      <c r="G1410" s="13"/>
+      <c r="J1410" s="13"/>
+      <c r="L1410" s="13"/>
+      <c r="M1410" s="13"/>
+      <c r="N1410" s="13"/>
     </row>
     <row r="1411" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1411" s="1" t="s">
@@ -71576,128 +71576,128 @@
         <v>3830</v>
       </c>
     </row>
-    <row r="1469" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1469" s="9"/>
-      <c r="B1469" s="10">
+    <row r="1469" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1469" s="13"/>
+      <c r="B1469" s="14">
         <v>12</v>
       </c>
-      <c r="C1469" s="9" t="s">
+      <c r="C1469" s="13" t="s">
         <v>4921</v>
       </c>
-      <c r="D1469" s="9" t="s">
+      <c r="D1469" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1469" s="9"/>
-      <c r="G1469" s="9">
+      <c r="F1469" s="13"/>
+      <c r="G1469" s="13">
         <v>100</v>
       </c>
-      <c r="I1469" s="10" t="s">
+      <c r="I1469" s="14" t="s">
         <v>4410</v>
       </c>
-      <c r="J1469" s="9"/>
-      <c r="L1469" s="9"/>
-      <c r="M1469" s="9"/>
-      <c r="N1469" s="9" t="s">
+      <c r="J1469" s="13"/>
+      <c r="L1469" s="13"/>
+      <c r="M1469" s="13"/>
+      <c r="N1469" s="13" t="s">
         <v>4922</v>
       </c>
     </row>
-    <row r="1470" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1470" s="9"/>
-      <c r="B1470" s="10">
+    <row r="1470" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1470" s="13"/>
+      <c r="B1470" s="14">
         <v>13</v>
       </c>
-      <c r="C1470" s="9" t="s">
+      <c r="C1470" s="13" t="s">
         <v>4923</v>
       </c>
-      <c r="D1470" s="9" t="s">
+      <c r="D1470" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1470" s="9"/>
-      <c r="G1470" s="9">
+      <c r="F1470" s="13"/>
+      <c r="G1470" s="13">
         <v>100</v>
       </c>
-      <c r="I1470" s="10" t="s">
+      <c r="I1470" s="14" t="s">
         <v>4412</v>
       </c>
-      <c r="J1470" s="9"/>
-      <c r="L1470" s="9"/>
-      <c r="M1470" s="9"/>
-      <c r="N1470" s="9" t="s">
+      <c r="J1470" s="13"/>
+      <c r="L1470" s="13"/>
+      <c r="M1470" s="13"/>
+      <c r="N1470" s="13" t="s">
         <v>4924</v>
       </c>
     </row>
-    <row r="1471" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1471" s="9"/>
-      <c r="B1471" s="10">
+    <row r="1471" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1471" s="13"/>
+      <c r="B1471" s="14">
         <v>14</v>
       </c>
-      <c r="C1471" s="9" t="s">
+      <c r="C1471" s="13" t="s">
         <v>4925</v>
       </c>
-      <c r="D1471" s="9" t="s">
+      <c r="D1471" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1471" s="9"/>
-      <c r="G1471" s="9">
+      <c r="F1471" s="13"/>
+      <c r="G1471" s="13">
         <v>100</v>
       </c>
-      <c r="I1471" s="10" t="s">
+      <c r="I1471" s="14" t="s">
         <v>4412</v>
       </c>
-      <c r="J1471" s="9"/>
-      <c r="L1471" s="9"/>
-      <c r="M1471" s="9"/>
-      <c r="N1471" s="9" t="s">
+      <c r="J1471" s="13"/>
+      <c r="L1471" s="13"/>
+      <c r="M1471" s="13"/>
+      <c r="N1471" s="13" t="s">
         <v>4926</v>
       </c>
     </row>
-    <row r="1472" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1472" s="9"/>
-      <c r="B1472" s="10">
+    <row r="1472" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1472" s="13"/>
+      <c r="B1472" s="14">
         <v>15</v>
       </c>
-      <c r="C1472" s="9" t="s">
+      <c r="C1472" s="13" t="s">
         <v>4927</v>
       </c>
-      <c r="D1472" s="9" t="s">
+      <c r="D1472" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="F1472" s="9"/>
-      <c r="G1472" s="9">
+      <c r="F1472" s="13"/>
+      <c r="G1472" s="13">
         <v>1000</v>
       </c>
-      <c r="I1472" s="10" t="s">
+      <c r="I1472" s="14" t="s">
         <v>3830</v>
       </c>
-      <c r="J1472" s="9"/>
-      <c r="L1472" s="9"/>
-      <c r="M1472" s="9"/>
-      <c r="N1472" s="9" t="s">
+      <c r="J1472" s="13"/>
+      <c r="L1472" s="13"/>
+      <c r="M1472" s="13"/>
+      <c r="N1472" s="13" t="s">
         <v>4928</v>
       </c>
     </row>
-    <row r="1473" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1473" s="9"/>
-      <c r="B1473" s="10">
+    <row r="1473" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1473" s="13"/>
+      <c r="B1473" s="14">
         <v>16</v>
       </c>
-      <c r="C1473" s="9" t="s">
+      <c r="C1473" s="13" t="s">
         <v>4929</v>
       </c>
-      <c r="D1473" s="9" t="s">
+      <c r="D1473" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="F1473" s="9"/>
-      <c r="G1473" s="9">
+      <c r="F1473" s="13"/>
+      <c r="G1473" s="13">
         <v>1000</v>
       </c>
-      <c r="I1473" s="10" t="s">
+      <c r="I1473" s="14" t="s">
         <v>3830</v>
       </c>
-      <c r="J1473" s="9"/>
-      <c r="L1473" s="9"/>
-      <c r="M1473" s="9"/>
-      <c r="N1473" s="9" t="s">
+      <c r="J1473" s="13"/>
+      <c r="L1473" s="13"/>
+      <c r="M1473" s="13"/>
+      <c r="N1473" s="13" t="s">
         <v>4930</v>
       </c>
     </row>
@@ -71835,476 +71835,476 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1481" spans="1:16" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1481" s="11" t="s">
+    <row r="1481" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1481" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="C1481" s="11"/>
-      <c r="D1481" s="11"/>
-      <c r="F1481" s="11"/>
-      <c r="G1481" s="11"/>
-      <c r="J1481" s="11"/>
-      <c r="L1481" s="11"/>
-      <c r="M1481" s="11"/>
-      <c r="N1481" s="11" t="s">
+      <c r="C1481" s="13"/>
+      <c r="D1481" s="13"/>
+      <c r="F1481" s="13"/>
+      <c r="G1481" s="13"/>
+      <c r="J1481" s="13"/>
+      <c r="L1481" s="13"/>
+      <c r="M1481" s="13"/>
+      <c r="N1481" s="13" t="s">
         <v>4942</v>
       </c>
-      <c r="P1481" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1482" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1482" s="9"/>
-      <c r="B1482" s="10">
+      <c r="P1481" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1482" s="13"/>
+      <c r="B1482" s="14">
         <v>253</v>
       </c>
-      <c r="C1482" s="9" t="s">
+      <c r="C1482" s="13" t="s">
         <v>3829</v>
       </c>
-      <c r="D1482" s="9" t="s">
+      <c r="D1482" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F1482" s="9"/>
-      <c r="G1482" s="9"/>
-      <c r="J1482" s="9"/>
-      <c r="L1482" s="9"/>
-      <c r="M1482" s="9"/>
-      <c r="N1482" s="9"/>
-    </row>
-    <row r="1483" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1483" s="9"/>
-      <c r="B1483" s="10">
+      <c r="F1482" s="13"/>
+      <c r="G1482" s="13"/>
+      <c r="J1482" s="13"/>
+      <c r="L1482" s="13"/>
+      <c r="M1482" s="13"/>
+      <c r="N1482" s="13"/>
+    </row>
+    <row r="1483" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1483" s="13"/>
+      <c r="B1483" s="14">
         <v>0</v>
       </c>
-      <c r="C1483" s="9" t="s">
+      <c r="C1483" s="13" t="s">
         <v>3840</v>
       </c>
-      <c r="D1483" s="9" t="s">
+      <c r="D1483" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1483" s="9"/>
-      <c r="G1483" s="9"/>
-      <c r="I1483" s="10" t="s">
+      <c r="F1483" s="13"/>
+      <c r="G1483" s="13"/>
+      <c r="I1483" s="14" t="s">
         <v>3841</v>
       </c>
-      <c r="J1483" s="9"/>
-      <c r="L1483" s="9"/>
-      <c r="M1483" s="9"/>
-      <c r="N1483" s="9" t="s">
+      <c r="J1483" s="13"/>
+      <c r="L1483" s="13"/>
+      <c r="M1483" s="13"/>
+      <c r="N1483" s="13" t="s">
         <v>4943</v>
       </c>
     </row>
-    <row r="1484" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1484" s="9"/>
-      <c r="B1484" s="10">
-        <v>1</v>
-      </c>
-      <c r="C1484" s="9" t="s">
+    <row r="1484" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1484" s="13"/>
+      <c r="B1484" s="14">
+        <v>1</v>
+      </c>
+      <c r="C1484" s="13" t="s">
         <v>654</v>
       </c>
-      <c r="D1484" s="9" t="s">
+      <c r="D1484" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E1484" s="10" t="s">
+      <c r="E1484" s="14" t="s">
         <v>3849</v>
       </c>
-      <c r="F1484" s="9"/>
-      <c r="G1484" s="9"/>
-      <c r="I1484" s="10" t="s">
+      <c r="F1484" s="13"/>
+      <c r="G1484" s="13"/>
+      <c r="I1484" s="14" t="s">
         <v>3841</v>
       </c>
-      <c r="J1484" s="9"/>
-      <c r="L1484" s="9"/>
-      <c r="M1484" s="9"/>
-      <c r="N1484" s="9" t="s">
+      <c r="J1484" s="13"/>
+      <c r="L1484" s="13"/>
+      <c r="M1484" s="13"/>
+      <c r="N1484" s="13" t="s">
         <v>4944</v>
       </c>
     </row>
-    <row r="1485" spans="1:16" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1485" s="11" t="s">
+    <row r="1485" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1485" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C1485" s="11"/>
-      <c r="D1485" s="11"/>
-      <c r="F1485" s="11"/>
-      <c r="G1485" s="11"/>
-      <c r="J1485" s="11"/>
-      <c r="L1485" s="11"/>
-      <c r="M1485" s="11"/>
-      <c r="N1485" s="11"/>
-    </row>
-    <row r="1486" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1486" s="9"/>
-      <c r="B1486" s="10">
+      <c r="C1485" s="13"/>
+      <c r="D1485" s="13"/>
+      <c r="F1485" s="13"/>
+      <c r="G1485" s="13"/>
+      <c r="J1485" s="13"/>
+      <c r="L1485" s="13"/>
+      <c r="M1485" s="13"/>
+      <c r="N1485" s="13"/>
+    </row>
+    <row r="1486" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1486" s="13"/>
+      <c r="B1486" s="14">
         <v>253</v>
       </c>
-      <c r="C1486" s="9" t="s">
+      <c r="C1486" s="13" t="s">
         <v>3829</v>
       </c>
-      <c r="D1486" s="9" t="s">
+      <c r="D1486" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F1486" s="9"/>
-      <c r="G1486" s="9"/>
-      <c r="J1486" s="9"/>
-      <c r="L1486" s="9"/>
-      <c r="M1486" s="9"/>
-      <c r="N1486" s="9"/>
-    </row>
-    <row r="1487" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1487" s="9"/>
-      <c r="B1487" s="10">
+      <c r="F1486" s="13"/>
+      <c r="G1486" s="13"/>
+      <c r="J1486" s="13"/>
+      <c r="L1486" s="13"/>
+      <c r="M1486" s="13"/>
+      <c r="N1486" s="13"/>
+    </row>
+    <row r="1487" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1487" s="13"/>
+      <c r="B1487" s="14">
         <v>0</v>
       </c>
-      <c r="C1487" s="9" t="s">
+      <c r="C1487" s="13" t="s">
         <v>4945</v>
       </c>
-      <c r="D1487" s="9" t="s">
+      <c r="D1487" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1487" s="9"/>
-      <c r="G1487" s="9">
+      <c r="F1487" s="13"/>
+      <c r="G1487" s="13">
         <v>128</v>
       </c>
-      <c r="I1487" s="10" t="s">
+      <c r="I1487" s="14" t="s">
         <v>3841</v>
       </c>
-      <c r="J1487" s="9"/>
-      <c r="L1487" s="9"/>
-      <c r="M1487" s="9"/>
-      <c r="N1487" s="9" t="s">
+      <c r="J1487" s="13"/>
+      <c r="L1487" s="13"/>
+      <c r="M1487" s="13"/>
+      <c r="N1487" s="13" t="s">
         <v>4946</v>
       </c>
     </row>
-    <row r="1488" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1488" s="9"/>
-      <c r="B1488" s="10">
-        <v>1</v>
-      </c>
-      <c r="C1488" s="9" t="s">
+    <row r="1488" spans="1:16" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1488" s="13"/>
+      <c r="B1488" s="14">
+        <v>1</v>
+      </c>
+      <c r="C1488" s="13" t="s">
         <v>4947</v>
       </c>
-      <c r="D1488" s="9" t="s">
+      <c r="D1488" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1488" s="9"/>
-      <c r="G1488" s="9">
+      <c r="F1488" s="13"/>
+      <c r="G1488" s="13">
         <v>128</v>
       </c>
-      <c r="I1488" s="10" t="s">
+      <c r="I1488" s="14" t="s">
         <v>3841</v>
       </c>
-      <c r="J1488" s="9"/>
-      <c r="L1488" s="9"/>
-      <c r="M1488" s="9"/>
-      <c r="N1488" s="9" t="s">
+      <c r="J1488" s="13"/>
+      <c r="L1488" s="13"/>
+      <c r="M1488" s="13"/>
+      <c r="N1488" s="13" t="s">
         <v>4948</v>
       </c>
     </row>
-    <row r="1489" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1489" s="9"/>
-      <c r="B1489" s="10">
+    <row r="1489" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1489" s="13"/>
+      <c r="B1489" s="14">
         <v>2</v>
       </c>
-      <c r="C1489" s="9" t="s">
+      <c r="C1489" s="13" t="s">
         <v>4949</v>
       </c>
-      <c r="D1489" s="9" t="s">
+      <c r="D1489" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1489" s="9"/>
-      <c r="G1489" s="9">
+      <c r="F1489" s="13"/>
+      <c r="G1489" s="13">
         <v>128</v>
       </c>
-      <c r="I1489" s="10" t="s">
+      <c r="I1489" s="14" t="s">
         <v>3841</v>
       </c>
-      <c r="J1489" s="9"/>
-      <c r="L1489" s="9"/>
-      <c r="M1489" s="9"/>
-      <c r="N1489" s="9" t="s">
+      <c r="J1489" s="13"/>
+      <c r="L1489" s="13"/>
+      <c r="M1489" s="13"/>
+      <c r="N1489" s="13" t="s">
         <v>4950</v>
       </c>
     </row>
-    <row r="1490" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1490" s="9"/>
-      <c r="B1490" s="10">
+    <row r="1490" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1490" s="13"/>
+      <c r="B1490" s="14">
         <v>3</v>
       </c>
-      <c r="C1490" s="9" t="s">
+      <c r="C1490" s="13" t="s">
         <v>4951</v>
       </c>
-      <c r="D1490" s="9" t="s">
+      <c r="D1490" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1490" s="9"/>
-      <c r="G1490" s="9">
+      <c r="F1490" s="13"/>
+      <c r="G1490" s="13">
         <v>128</v>
       </c>
-      <c r="I1490" s="10" t="s">
+      <c r="I1490" s="14" t="s">
         <v>3841</v>
       </c>
-      <c r="J1490" s="9"/>
-      <c r="L1490" s="9"/>
-      <c r="M1490" s="9"/>
-      <c r="N1490" s="9" t="s">
+      <c r="J1490" s="13"/>
+      <c r="L1490" s="13"/>
+      <c r="M1490" s="13"/>
+      <c r="N1490" s="13" t="s">
         <v>4952</v>
       </c>
     </row>
-    <row r="1491" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1491" s="9"/>
-      <c r="B1491" s="10">
+    <row r="1491" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1491" s="13"/>
+      <c r="B1491" s="14">
         <v>4</v>
       </c>
-      <c r="C1491" s="9" t="s">
+      <c r="C1491" s="13" t="s">
         <v>4953</v>
       </c>
-      <c r="D1491" s="9" t="s">
+      <c r="D1491" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1491" s="9"/>
-      <c r="G1491" s="9">
+      <c r="F1491" s="13"/>
+      <c r="G1491" s="13">
         <v>128</v>
       </c>
-      <c r="I1491" s="10" t="s">
+      <c r="I1491" s="14" t="s">
         <v>3841</v>
       </c>
-      <c r="J1491" s="9"/>
-      <c r="L1491" s="9"/>
-      <c r="M1491" s="9"/>
-      <c r="N1491" s="9" t="s">
+      <c r="J1491" s="13"/>
+      <c r="L1491" s="13"/>
+      <c r="M1491" s="13"/>
+      <c r="N1491" s="13" t="s">
         <v>4954</v>
       </c>
     </row>
-    <row r="1492" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1492" s="9"/>
-      <c r="B1492" s="10">
+    <row r="1492" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1492" s="13"/>
+      <c r="B1492" s="14">
         <v>5</v>
       </c>
-      <c r="C1492" s="9" t="s">
+      <c r="C1492" s="13" t="s">
         <v>4955</v>
       </c>
-      <c r="D1492" s="9" t="s">
+      <c r="D1492" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1492" s="9"/>
-      <c r="G1492" s="9">
+      <c r="F1492" s="13"/>
+      <c r="G1492" s="13">
         <v>128</v>
       </c>
-      <c r="I1492" s="10" t="s">
+      <c r="I1492" s="14" t="s">
         <v>3841</v>
       </c>
-      <c r="J1492" s="9"/>
-      <c r="L1492" s="9"/>
-      <c r="M1492" s="9"/>
-      <c r="N1492" s="9" t="s">
+      <c r="J1492" s="13"/>
+      <c r="L1492" s="13"/>
+      <c r="M1492" s="13"/>
+      <c r="N1492" s="13" t="s">
         <v>4956</v>
       </c>
     </row>
-    <row r="1493" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1493" s="9"/>
-      <c r="B1493" s="10">
+    <row r="1493" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1493" s="13"/>
+      <c r="B1493" s="14">
         <v>6</v>
       </c>
-      <c r="C1493" s="9" t="s">
+      <c r="C1493" s="13" t="s">
         <v>4086</v>
       </c>
-      <c r="D1493" s="9" t="s">
+      <c r="D1493" s="13" t="s">
         <v>3791</v>
       </c>
-      <c r="F1493" s="9"/>
-      <c r="G1493" s="9"/>
-      <c r="J1493" s="9"/>
-      <c r="L1493" s="9"/>
-      <c r="M1493" s="9"/>
-      <c r="N1493" s="9"/>
-    </row>
-    <row r="1494" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1494" s="11" t="s">
+      <c r="F1493" s="13"/>
+      <c r="G1493" s="13"/>
+      <c r="J1493" s="13"/>
+      <c r="L1493" s="13"/>
+      <c r="M1493" s="13"/>
+      <c r="N1493" s="13"/>
+    </row>
+    <row r="1494" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1494" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C1494" s="11"/>
-      <c r="D1494" s="11"/>
-      <c r="F1494" s="11"/>
-      <c r="G1494" s="11"/>
-      <c r="J1494" s="11"/>
-      <c r="L1494" s="11"/>
-      <c r="M1494" s="11"/>
-      <c r="N1494" s="11"/>
-    </row>
-    <row r="1495" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1495" s="9"/>
-      <c r="B1495" s="10">
+      <c r="C1494" s="13"/>
+      <c r="D1494" s="13"/>
+      <c r="F1494" s="13"/>
+      <c r="G1494" s="13"/>
+      <c r="J1494" s="13"/>
+      <c r="L1494" s="13"/>
+      <c r="M1494" s="13"/>
+      <c r="N1494" s="13"/>
+    </row>
+    <row r="1495" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1495" s="13"/>
+      <c r="B1495" s="14">
         <v>253</v>
       </c>
-      <c r="C1495" s="9" t="s">
+      <c r="C1495" s="13" t="s">
         <v>3829</v>
       </c>
-      <c r="D1495" s="9" t="s">
+      <c r="D1495" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F1495" s="9"/>
-      <c r="G1495" s="9"/>
-      <c r="J1495" s="9"/>
-      <c r="L1495" s="9"/>
-      <c r="M1495" s="9"/>
-      <c r="N1495" s="9"/>
-    </row>
-    <row r="1496" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1496" s="9"/>
-      <c r="B1496" s="10">
+      <c r="F1495" s="13"/>
+      <c r="G1495" s="13"/>
+      <c r="J1495" s="13"/>
+      <c r="L1495" s="13"/>
+      <c r="M1495" s="13"/>
+      <c r="N1495" s="13"/>
+    </row>
+    <row r="1496" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1496" s="13"/>
+      <c r="B1496" s="14">
         <v>0</v>
       </c>
-      <c r="C1496" s="9" t="s">
+      <c r="C1496" s="13" t="s">
         <v>4090</v>
       </c>
-      <c r="D1496" s="9" t="s">
+      <c r="D1496" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1496" s="9"/>
-      <c r="G1496" s="9">
+      <c r="F1496" s="13"/>
+      <c r="G1496" s="13">
         <v>128</v>
       </c>
-      <c r="I1496" s="10" t="s">
+      <c r="I1496" s="14" t="s">
         <v>3841</v>
       </c>
-      <c r="J1496" s="9"/>
-      <c r="L1496" s="9"/>
-      <c r="M1496" s="9"/>
-      <c r="N1496" s="9" t="s">
+      <c r="J1496" s="13"/>
+      <c r="L1496" s="13"/>
+      <c r="M1496" s="13"/>
+      <c r="N1496" s="13" t="s">
         <v>4957</v>
       </c>
     </row>
-    <row r="1497" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1497" s="11" t="s">
+    <row r="1497" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1497" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C1497" s="11"/>
-      <c r="D1497" s="11"/>
-      <c r="F1497" s="11"/>
-      <c r="G1497" s="11"/>
-      <c r="J1497" s="11"/>
-      <c r="L1497" s="11"/>
-      <c r="M1497" s="11"/>
-      <c r="N1497" s="11"/>
-    </row>
-    <row r="1498" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1498" s="9"/>
-      <c r="B1498" s="10">
+      <c r="C1497" s="13"/>
+      <c r="D1497" s="13"/>
+      <c r="F1497" s="13"/>
+      <c r="G1497" s="13"/>
+      <c r="J1497" s="13"/>
+      <c r="L1497" s="13"/>
+      <c r="M1497" s="13"/>
+      <c r="N1497" s="13"/>
+    </row>
+    <row r="1498" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1498" s="13"/>
+      <c r="B1498" s="14">
         <v>253</v>
       </c>
-      <c r="C1498" s="9" t="s">
+      <c r="C1498" s="13" t="s">
         <v>3829</v>
       </c>
-      <c r="D1498" s="9" t="s">
+      <c r="D1498" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F1498" s="9"/>
-      <c r="G1498" s="9"/>
-      <c r="J1498" s="9"/>
-      <c r="L1498" s="9"/>
-      <c r="M1498" s="9"/>
-      <c r="N1498" s="9"/>
-    </row>
-    <row r="1499" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1499" s="9"/>
-      <c r="B1499" s="10">
+      <c r="F1498" s="13"/>
+      <c r="G1498" s="13"/>
+      <c r="J1498" s="13"/>
+      <c r="L1498" s="13"/>
+      <c r="M1498" s="13"/>
+      <c r="N1498" s="13"/>
+    </row>
+    <row r="1499" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1499" s="13"/>
+      <c r="B1499" s="14">
         <v>0</v>
       </c>
-      <c r="C1499" s="9" t="s">
+      <c r="C1499" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="D1499" s="9" t="s">
+      <c r="D1499" s="13" t="s">
         <v>2316</v>
       </c>
-      <c r="F1499" s="9"/>
-      <c r="G1499" s="9">
+      <c r="F1499" s="13"/>
+      <c r="G1499" s="13">
         <v>100</v>
       </c>
-      <c r="I1499" s="10" t="s">
+      <c r="I1499" s="14" t="s">
         <v>4958</v>
       </c>
-      <c r="J1499" s="9"/>
-      <c r="L1499" s="9"/>
-      <c r="M1499" s="9"/>
-      <c r="N1499" s="9" t="s">
+      <c r="J1499" s="13"/>
+      <c r="L1499" s="13"/>
+      <c r="M1499" s="13"/>
+      <c r="N1499" s="13" t="s">
         <v>4959</v>
       </c>
     </row>
-    <row r="1500" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1500" s="11" t="s">
+    <row r="1500" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1500" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C1500" s="11"/>
-      <c r="D1500" s="11"/>
-      <c r="F1500" s="11"/>
-      <c r="G1500" s="11"/>
-      <c r="J1500" s="11"/>
-      <c r="L1500" s="11"/>
-      <c r="M1500" s="11"/>
-      <c r="N1500" s="11"/>
-    </row>
-    <row r="1501" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1501" s="9"/>
-      <c r="B1501" s="10">
+      <c r="C1500" s="13"/>
+      <c r="D1500" s="13"/>
+      <c r="F1500" s="13"/>
+      <c r="G1500" s="13"/>
+      <c r="J1500" s="13"/>
+      <c r="L1500" s="13"/>
+      <c r="M1500" s="13"/>
+      <c r="N1500" s="13"/>
+    </row>
+    <row r="1501" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1501" s="13"/>
+      <c r="B1501" s="14">
         <v>253</v>
       </c>
-      <c r="C1501" s="9" t="s">
+      <c r="C1501" s="13" t="s">
         <v>3829</v>
       </c>
-      <c r="D1501" s="9" t="s">
+      <c r="D1501" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F1501" s="9"/>
-      <c r="G1501" s="9"/>
-      <c r="I1501" s="10" t="s">
+      <c r="F1501" s="13"/>
+      <c r="G1501" s="13"/>
+      <c r="I1501" s="14" t="s">
         <v>3830</v>
       </c>
-      <c r="J1501" s="9"/>
-      <c r="L1501" s="9"/>
-      <c r="M1501" s="9"/>
-      <c r="N1501" s="9"/>
-    </row>
-    <row r="1502" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1502" s="9"/>
-      <c r="B1502" s="10">
+      <c r="J1501" s="13"/>
+      <c r="L1501" s="13"/>
+      <c r="M1501" s="13"/>
+      <c r="N1501" s="13"/>
+    </row>
+    <row r="1502" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1502" s="13"/>
+      <c r="B1502" s="14">
         <v>0</v>
       </c>
-      <c r="C1502" s="9" t="s">
+      <c r="C1502" s="13" t="s">
         <v>4960</v>
       </c>
-      <c r="D1502" s="9" t="s">
+      <c r="D1502" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F1502" s="9"/>
-      <c r="G1502" s="9"/>
-      <c r="J1502" s="9"/>
-      <c r="L1502" s="9"/>
-      <c r="M1502" s="9"/>
-      <c r="N1502" s="9"/>
-    </row>
-    <row r="1503" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1503" s="9"/>
-      <c r="B1503" s="10">
-        <v>1</v>
-      </c>
-      <c r="C1503" s="9" t="s">
+      <c r="F1502" s="13"/>
+      <c r="G1502" s="13"/>
+      <c r="J1502" s="13"/>
+      <c r="L1502" s="13"/>
+      <c r="M1502" s="13"/>
+      <c r="N1502" s="13"/>
+    </row>
+    <row r="1503" spans="1:14" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1503" s="13"/>
+      <c r="B1503" s="14">
+        <v>1</v>
+      </c>
+      <c r="C1503" s="13" t="s">
         <v>2310</v>
       </c>
-      <c r="D1503" s="9" t="s">
+      <c r="D1503" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1503" s="9"/>
-      <c r="G1503" s="9">
+      <c r="F1503" s="13"/>
+      <c r="G1503" s="13">
         <v>100</v>
       </c>
-      <c r="I1503" s="10" t="s">
+      <c r="I1503" s="14" t="s">
         <v>2135</v>
       </c>
-      <c r="J1503" s="9"/>
-      <c r="L1503" s="9"/>
-      <c r="M1503" s="9"/>
-      <c r="N1503" s="9"/>
+      <c r="J1503" s="13"/>
+      <c r="L1503" s="13"/>
+      <c r="M1503" s="13"/>
+      <c r="N1503" s="13"/>
     </row>
     <row r="1504" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1504" s="11" t="s">

</xml_diff>